<commit_message>
Added check and wait if the previous frame is still calculating/rendering
Also added a one frame delay when switching scenarios to give worker threads time to finish. Updated README.md and Notes.md with more details.
</commit_message>
<xml_diff>
--- a/Design and Notes/UWP Version Performance.xlsx
+++ b/Design and Notes/UWP Version Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezoch\Repos\Gravity-Sandbox\Design and Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D390EF7-1770-4EFD-A6CB-3E9DAAFE6A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345ED2C2-2C3D-4642-B15B-CF4EA996508D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="6255" windowWidth="27765" windowHeight="15105" xr2:uid="{E3490D73-55F9-4282-B919-40936295C062}"/>
+    <workbookView xWindow="3570" yWindow="8295" windowWidth="27765" windowHeight="15105" xr2:uid="{E3490D73-55F9-4282-B919-40936295C062}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -111,16 +111,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -436,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCE57E2-F661-4537-A914-B4C74C70A528}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E19" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +479,7 @@
         <v>67</v>
       </c>
       <c r="E2" s="2">
-        <f>A2*A2</f>
+        <f t="shared" ref="E2:E8" si="0">A2*A2</f>
         <v>100</v>
       </c>
       <c r="F2" s="3"/>
@@ -498,7 +499,7 @@
         <v>71</v>
       </c>
       <c r="E3" s="2">
-        <f>A3*A3</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="F3" s="3"/>
@@ -515,7 +516,7 @@
         <v>11.1</v>
       </c>
       <c r="E4" s="2">
-        <f>A4*A4</f>
+        <f t="shared" si="0"/>
         <v>22500</v>
       </c>
       <c r="F4" s="3"/>
@@ -532,7 +533,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="2">
-        <f>A5*A5</f>
+        <f t="shared" si="0"/>
         <v>62500</v>
       </c>
       <c r="F5" s="3"/>
@@ -549,7 +550,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="2">
-        <f>A6*A6</f>
+        <f t="shared" si="0"/>
         <v>90000</v>
       </c>
       <c r="F6" s="3"/>
@@ -566,7 +567,7 @@
         <v>62</v>
       </c>
       <c r="E7" s="2">
-        <f>A7*A7</f>
+        <f t="shared" si="0"/>
         <v>250000</v>
       </c>
       <c r="F7" s="3"/>
@@ -583,7 +584,7 @@
         <v>194</v>
       </c>
       <c r="E8" s="2">
-        <f>A8*A8</f>
+        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
       <c r="F8" s="3"/>
@@ -660,6 +661,70 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>SQRT(E17)</f>
+        <v>701.560760020114</v>
+      </c>
+      <c r="B17" s="3">
+        <f>C$13*C17 - 15</f>
+        <v>78.75</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="7">
+        <f>B17/B$7*E$7</f>
+        <v>492187.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" ref="A18:A20" si="1">SQRT(E18)</f>
+        <v>829.15619758884998</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" ref="B18:B19" si="2">C$13*C18 - 15</f>
+        <v>110</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" ref="E18:E20" si="3">B18/B$7*E$7</f>
+        <v>687500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>939.58102364830677</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="2"/>
+        <v>141.25</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="3"/>
+        <v>882812.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>418.33001326703777</v>
+      </c>
+      <c r="B20">
+        <v>28</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="3"/>
+        <v>175000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>